<commit_message>
Update EIA data to 2017
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/EIA-data/Table_6.2_Coal_Consumption_by_Sector.xlsx
+++ b/input/emissions-inventories/EIA-data/Table_6.2_Coal_Consumption_by_Sector.xlsx
@@ -21,13 +21,13 @@
     <t>U.S. Energy Information Administration</t>
   </si>
   <si>
-    <t>May 2017 Monthly Energy Review</t>
+    <t>June 2018 Monthly Energy Review</t>
   </si>
   <si>
-    <t>Release Date: May 25, 2017</t>
+    <t>Release Date: June 26, 2018</t>
   </si>
   <si>
-    <t>Next Update: June 28, 2017</t>
+    <t>Next Update: July 26, 2018</t>
   </si>
   <si>
     <t>Table 6.2 Coal Consumption by Sector</t>
@@ -485,7 +485,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M542"/>
+  <dimension ref="A1:M555"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -21783,37 +21783,37 @@
         <v>19</v>
       </c>
       <c r="C529">
-        <v>75.589</v>
+        <v>75.262</v>
       </c>
       <c r="D529">
-        <v>72.72</v>
+        <v>74.912</v>
       </c>
       <c r="E529">
-        <v>148.309</v>
+        <v>150.174</v>
       </c>
       <c r="F529">
         <v>1328.483</v>
       </c>
       <c r="G529">
-        <v>1503.052</v>
+        <v>1397.261</v>
       </c>
       <c r="H529">
-        <v>1533.252</v>
+        <v>1651.675</v>
       </c>
       <c r="I529">
-        <v>3036.304</v>
+        <v>3048.936</v>
       </c>
       <c r="J529">
-        <v>4364.787</v>
+        <v>4377.419</v>
       </c>
       <c r="K529">
         <v>0</v>
       </c>
       <c r="L529">
-        <v>61969.945</v>
+        <v>62134.631</v>
       </c>
       <c r="M529">
-        <v>66483.041</v>
+        <v>66662.224</v>
       </c>
     </row>
     <row r="530" spans="1:13">
@@ -21824,37 +21824,37 @@
         <v>19</v>
       </c>
       <c r="C530">
-        <v>77.956</v>
+        <v>75.387</v>
       </c>
       <c r="D530">
-        <v>74.997</v>
+        <v>75.036</v>
       </c>
       <c r="E530">
-        <v>152.953</v>
+        <v>150.423</v>
       </c>
       <c r="F530">
         <v>1361.445</v>
       </c>
       <c r="G530">
-        <v>1395.111</v>
+        <v>1282.036</v>
       </c>
       <c r="H530">
-        <v>1629.704</v>
+        <v>1755.363</v>
       </c>
       <c r="I530">
-        <v>3024.815</v>
+        <v>3037.399</v>
       </c>
       <c r="J530">
-        <v>4386.26</v>
+        <v>4398.844</v>
       </c>
       <c r="K530">
         <v>0</v>
       </c>
       <c r="L530">
-        <v>50487.225</v>
+        <v>50661.45</v>
       </c>
       <c r="M530">
-        <v>55026.438</v>
+        <v>55210.717</v>
       </c>
     </row>
     <row r="531" spans="1:13">
@@ -21865,37 +21865,37 @@
         <v>19</v>
       </c>
       <c r="C531">
-        <v>74.92</v>
+        <v>74.003</v>
       </c>
       <c r="D531">
-        <v>72.076</v>
+        <v>73.658</v>
       </c>
       <c r="E531">
-        <v>146.996</v>
+        <v>147.661</v>
       </c>
       <c r="F531">
         <v>1433.657</v>
       </c>
       <c r="G531">
-        <v>1369.91</v>
+        <v>1274.833</v>
       </c>
       <c r="H531">
-        <v>1662.617</v>
+        <v>1770.31</v>
       </c>
       <c r="I531">
-        <v>3032.527</v>
+        <v>3045.143</v>
       </c>
       <c r="J531">
-        <v>4466.184</v>
+        <v>4478.8</v>
       </c>
       <c r="K531">
         <v>0</v>
       </c>
       <c r="L531">
-        <v>39787.738</v>
+        <v>39948.145</v>
       </c>
       <c r="M531">
-        <v>44400.918</v>
+        <v>44574.606</v>
       </c>
     </row>
     <row r="532" spans="1:13">
@@ -21906,37 +21906,37 @@
         <v>19</v>
       </c>
       <c r="C532">
-        <v>49.432</v>
+        <v>45.553</v>
       </c>
       <c r="D532">
-        <v>26.85</v>
+        <v>28.657</v>
       </c>
       <c r="E532">
-        <v>76.282</v>
+        <v>74.21</v>
       </c>
       <c r="F532">
         <v>1324.031</v>
       </c>
       <c r="G532">
-        <v>1005.525</v>
+        <v>1075.583</v>
       </c>
       <c r="H532">
-        <v>1796.224</v>
+        <v>1750.917</v>
       </c>
       <c r="I532">
-        <v>2801.749</v>
+        <v>2826.5</v>
       </c>
       <c r="J532">
-        <v>4125.78</v>
+        <v>4150.531</v>
       </c>
       <c r="K532">
         <v>0</v>
       </c>
       <c r="L532">
-        <v>38983.58</v>
+        <v>39158.963</v>
       </c>
       <c r="M532">
-        <v>43185.642</v>
+        <v>43383.704</v>
       </c>
     </row>
     <row r="533" spans="1:13">
@@ -21947,37 +21947,37 @@
         <v>19</v>
       </c>
       <c r="C533">
-        <v>40.053</v>
+        <v>36.542</v>
       </c>
       <c r="D533">
-        <v>21.756</v>
+        <v>22.989</v>
       </c>
       <c r="E533">
-        <v>61.809</v>
+        <v>59.531</v>
       </c>
       <c r="F533">
         <v>1366.87</v>
       </c>
       <c r="G533">
-        <v>1148.66</v>
+        <v>1178.029</v>
       </c>
       <c r="H533">
-        <v>1661.116</v>
+        <v>1656.568</v>
       </c>
       <c r="I533">
-        <v>2809.776</v>
+        <v>2834.597</v>
       </c>
       <c r="J533">
-        <v>4176.646</v>
+        <v>4201.467</v>
       </c>
       <c r="K533">
         <v>0</v>
       </c>
       <c r="L533">
-        <v>44982.51</v>
+        <v>45081.935</v>
       </c>
       <c r="M533">
-        <v>49220.965</v>
+        <v>49342.933</v>
       </c>
     </row>
     <row r="534" spans="1:13">
@@ -21988,37 +21988,37 @@
         <v>19</v>
       </c>
       <c r="C534">
-        <v>46.125</v>
+        <v>46.166</v>
       </c>
       <c r="D534">
-        <v>25.054</v>
+        <v>29.043</v>
       </c>
       <c r="E534">
-        <v>71.179</v>
+        <v>75.209</v>
       </c>
       <c r="F534">
         <v>1404.818</v>
       </c>
       <c r="G534">
-        <v>1212.064</v>
+        <v>1242.702</v>
       </c>
       <c r="H534">
-        <v>1584.024</v>
+        <v>1578.086</v>
       </c>
       <c r="I534">
-        <v>2796.088</v>
+        <v>2820.788</v>
       </c>
       <c r="J534">
-        <v>4200.906</v>
+        <v>4225.606</v>
       </c>
       <c r="K534">
         <v>0</v>
       </c>
       <c r="L534">
-        <v>63243.408</v>
+        <v>63250.414</v>
       </c>
       <c r="M534">
-        <v>67515.493</v>
+        <v>67551.229</v>
       </c>
     </row>
     <row r="535" spans="1:13">
@@ -22029,37 +22029,37 @@
         <v>19</v>
       </c>
       <c r="C535">
-        <v>45.911</v>
+        <v>46.143</v>
       </c>
       <c r="D535">
-        <v>17.13</v>
+        <v>17.383</v>
       </c>
       <c r="E535">
-        <v>63.041</v>
+        <v>63.526</v>
       </c>
       <c r="F535">
         <v>1432.54</v>
       </c>
       <c r="G535">
-        <v>1234.352</v>
+        <v>1321.161</v>
       </c>
       <c r="H535">
-        <v>1578.068</v>
+        <v>1514.584</v>
       </c>
       <c r="I535">
-        <v>2812.42</v>
+        <v>2835.745</v>
       </c>
       <c r="J535">
-        <v>4244.96</v>
+        <v>4268.285</v>
       </c>
       <c r="K535">
         <v>0</v>
       </c>
       <c r="L535">
-        <v>74136.211</v>
+        <v>74236.728</v>
       </c>
       <c r="M535">
-        <v>78444.212</v>
+        <v>78568.539</v>
       </c>
     </row>
     <row r="536" spans="1:13">
@@ -22070,37 +22070,37 @@
         <v>19</v>
       </c>
       <c r="C536">
-        <v>50.489</v>
+        <v>49.413</v>
       </c>
       <c r="D536">
-        <v>18.838</v>
+        <v>18.615</v>
       </c>
       <c r="E536">
-        <v>69.327</v>
+        <v>68.028</v>
       </c>
       <c r="F536">
         <v>1394.678</v>
       </c>
       <c r="G536">
-        <v>1234.055</v>
+        <v>1292.162</v>
       </c>
       <c r="H536">
-        <v>1564.634</v>
+        <v>1529.738</v>
       </c>
       <c r="I536">
-        <v>2798.689</v>
+        <v>2821.9</v>
       </c>
       <c r="J536">
-        <v>4193.367</v>
+        <v>4216.578</v>
       </c>
       <c r="K536">
         <v>0</v>
       </c>
       <c r="L536">
-        <v>73756.853</v>
+        <v>73889.93</v>
       </c>
       <c r="M536">
-        <v>78019.547</v>
+        <v>78174.536</v>
       </c>
     </row>
     <row r="537" spans="1:13">
@@ -22111,37 +22111,37 @@
         <v>19</v>
       </c>
       <c r="C537">
-        <v>49.145</v>
+        <v>49.607</v>
       </c>
       <c r="D537">
-        <v>18.336</v>
+        <v>18.688</v>
       </c>
       <c r="E537">
-        <v>67.481</v>
+        <v>68.295</v>
       </c>
       <c r="F537">
         <v>1335.799</v>
       </c>
       <c r="G537">
-        <v>1053.123</v>
+        <v>1157.257</v>
       </c>
       <c r="H537">
-        <v>1749.224</v>
+        <v>1668.331</v>
       </c>
       <c r="I537">
-        <v>2802.347</v>
+        <v>2825.588</v>
       </c>
       <c r="J537">
-        <v>4138.146</v>
+        <v>4161.387</v>
       </c>
       <c r="K537">
         <v>0</v>
       </c>
       <c r="L537">
-        <v>62366.482</v>
+        <v>62385.216</v>
       </c>
       <c r="M537">
-        <v>66572.109</v>
+        <v>66614.898</v>
       </c>
     </row>
     <row r="538" spans="1:13">
@@ -22152,37 +22152,37 @@
         <v>19</v>
       </c>
       <c r="C538">
-        <v>49.717</v>
+        <v>49.856</v>
       </c>
       <c r="D538">
-        <v>38.787</v>
+        <v>37.991</v>
       </c>
       <c r="E538">
-        <v>88.504</v>
+        <v>87.847</v>
       </c>
       <c r="F538">
         <v>1334.67</v>
       </c>
       <c r="G538">
-        <v>992.665</v>
+        <v>1126.246</v>
       </c>
       <c r="H538">
-        <v>1880.306</v>
+        <v>1782.495</v>
       </c>
       <c r="I538">
-        <v>2872.971</v>
+        <v>2908.741</v>
       </c>
       <c r="J538">
-        <v>4207.641</v>
+        <v>4243.411</v>
       </c>
       <c r="K538">
         <v>0</v>
       </c>
       <c r="L538">
-        <v>54600.992</v>
+        <v>54621.445</v>
       </c>
       <c r="M538">
-        <v>58897.137</v>
+        <v>58952.703</v>
       </c>
     </row>
     <row r="539" spans="1:13">
@@ -22193,37 +22193,37 @@
         <v>19</v>
       </c>
       <c r="C539">
-        <v>61.191</v>
+        <v>59.538</v>
       </c>
       <c r="D539">
-        <v>47.739</v>
+        <v>45.368</v>
       </c>
       <c r="E539">
-        <v>108.93</v>
+        <v>104.906</v>
       </c>
       <c r="F539">
         <v>1325.968</v>
       </c>
       <c r="G539">
-        <v>998.442</v>
+        <v>1092.706</v>
       </c>
       <c r="H539">
-        <v>1888.775</v>
+        <v>1830.459</v>
       </c>
       <c r="I539">
-        <v>2887.217</v>
+        <v>2923.165</v>
       </c>
       <c r="J539">
-        <v>4213.185</v>
+        <v>4249.133</v>
       </c>
       <c r="K539">
         <v>0</v>
       </c>
       <c r="L539">
-        <v>48101.978</v>
+        <v>48179.203</v>
       </c>
       <c r="M539">
-        <v>52424.093</v>
+        <v>52533.242</v>
       </c>
     </row>
     <row r="540" spans="1:13">
@@ -22234,37 +22234,37 @@
         <v>19</v>
       </c>
       <c r="C540">
-        <v>71.392</v>
+        <v>75.425</v>
       </c>
       <c r="D540">
-        <v>55.697</v>
+        <v>57.474</v>
       </c>
       <c r="E540">
-        <v>127.089</v>
+        <v>132.899</v>
       </c>
       <c r="F540">
         <v>1441.749</v>
       </c>
       <c r="G540">
-        <v>1155.128</v>
+        <v>1280.244</v>
       </c>
       <c r="H540">
-        <v>1729.245</v>
+        <v>1640.041</v>
       </c>
       <c r="I540">
-        <v>2884.373</v>
+        <v>2920.285</v>
       </c>
       <c r="J540">
-        <v>4326.122</v>
+        <v>4362.034</v>
       </c>
       <c r="K540">
         <v>0</v>
       </c>
       <c r="L540">
-        <v>64857.805</v>
+        <v>65006.425</v>
       </c>
       <c r="M540">
-        <v>69311.016</v>
+        <v>69501.358</v>
       </c>
     </row>
     <row r="541" spans="1:13">
@@ -22275,37 +22275,37 @@
         <v>19</v>
       </c>
       <c r="C541">
-        <v>62.083</v>
+        <v>66.184</v>
       </c>
       <c r="D541">
-        <v>71.43</v>
+        <v>72.161</v>
       </c>
       <c r="E541">
-        <v>133.513</v>
+        <v>138.345</v>
       </c>
       <c r="F541">
-        <v>1553.584</v>
+        <v>1430.645</v>
       </c>
       <c r="G541">
-        <v>1287.693</v>
+        <v>1290.391</v>
       </c>
       <c r="H541">
-        <v>1720.253</v>
+        <v>1553.562</v>
       </c>
       <c r="I541">
-        <v>3007.946</v>
+        <v>2843.953</v>
       </c>
       <c r="J541">
-        <v>4561.53</v>
+        <v>4274.598</v>
       </c>
       <c r="K541">
         <v>0</v>
       </c>
       <c r="L541">
-        <v>63477.037</v>
+        <v>63547.714</v>
       </c>
       <c r="M541">
-        <v>68172.08</v>
+        <v>67960.657</v>
       </c>
     </row>
     <row r="542" spans="1:13">
@@ -22316,37 +22316,570 @@
         <v>19</v>
       </c>
       <c r="C542">
-        <v>50.257</v>
+        <v>53.674</v>
       </c>
       <c r="D542">
-        <v>50.579</v>
+        <v>58.521</v>
       </c>
       <c r="E542">
-        <v>100.836</v>
+        <v>112.195</v>
       </c>
       <c r="F542">
-        <v>1369.92</v>
+        <v>1367.727</v>
       </c>
       <c r="G542">
-        <v>1084.765</v>
+        <v>1087.427</v>
       </c>
       <c r="H542">
-        <v>1793.501</v>
+        <v>1766.993</v>
       </c>
       <c r="I542">
-        <v>2878.266</v>
+        <v>2854.42</v>
       </c>
       <c r="J542">
-        <v>4248.185</v>
+        <v>4222.147</v>
       </c>
       <c r="K542">
         <v>0</v>
       </c>
       <c r="L542">
-        <v>48094.506</v>
+        <v>47964.848</v>
       </c>
       <c r="M542">
-        <v>52443.527</v>
+        <v>52299.19</v>
+      </c>
+    </row>
+    <row r="543" spans="1:13">
+      <c r="A543" s="6">
+        <v>42795</v>
+      </c>
+      <c r="B543" t="s">
+        <v>19</v>
+      </c>
+      <c r="C543">
+        <v>58.423</v>
+      </c>
+      <c r="D543">
+        <v>63.699</v>
+      </c>
+      <c r="E543">
+        <v>122.122</v>
+      </c>
+      <c r="F543">
+        <v>1437.669</v>
+      </c>
+      <c r="G543">
+        <v>1172.172</v>
+      </c>
+      <c r="H543">
+        <v>1664.293</v>
+      </c>
+      <c r="I543">
+        <v>2836.465</v>
+      </c>
+      <c r="J543">
+        <v>4274.134</v>
+      </c>
+      <c r="K543">
+        <v>0</v>
+      </c>
+      <c r="L543">
+        <v>48825.958</v>
+      </c>
+      <c r="M543">
+        <v>53222.214</v>
+      </c>
+    </row>
+    <row r="544" spans="1:13">
+      <c r="A544" s="6">
+        <v>42826</v>
+      </c>
+      <c r="B544" t="s">
+        <v>19</v>
+      </c>
+      <c r="C544">
+        <v>40.473</v>
+      </c>
+      <c r="D544">
+        <v>24.9</v>
+      </c>
+      <c r="E544">
+        <v>65.373</v>
+      </c>
+      <c r="F544">
+        <v>1440.81</v>
+      </c>
+      <c r="G544">
+        <v>1067.605</v>
+      </c>
+      <c r="H544">
+        <v>1629.855</v>
+      </c>
+      <c r="I544">
+        <v>2697.46</v>
+      </c>
+      <c r="J544">
+        <v>4138.27</v>
+      </c>
+      <c r="K544">
+        <v>0</v>
+      </c>
+      <c r="L544">
+        <v>44323.847</v>
+      </c>
+      <c r="M544">
+        <v>48527.49</v>
+      </c>
+    </row>
+    <row r="545" spans="1:13">
+      <c r="A545" s="6">
+        <v>42856</v>
+      </c>
+      <c r="B545" t="s">
+        <v>19</v>
+      </c>
+      <c r="C545">
+        <v>39.962</v>
+      </c>
+      <c r="D545">
+        <v>24.586</v>
+      </c>
+      <c r="E545">
+        <v>64.548</v>
+      </c>
+      <c r="F545">
+        <v>1482.486</v>
+      </c>
+      <c r="G545">
+        <v>1098.283</v>
+      </c>
+      <c r="H545">
+        <v>1604.724</v>
+      </c>
+      <c r="I545">
+        <v>2703.007</v>
+      </c>
+      <c r="J545">
+        <v>4185.493</v>
+      </c>
+      <c r="K545">
+        <v>0</v>
+      </c>
+      <c r="L545">
+        <v>50926.005</v>
+      </c>
+      <c r="M545">
+        <v>55176.046</v>
+      </c>
+    </row>
+    <row r="546" spans="1:13">
+      <c r="A546" s="6">
+        <v>42887</v>
+      </c>
+      <c r="B546" t="s">
+        <v>19</v>
+      </c>
+      <c r="C546">
+        <v>45.507</v>
+      </c>
+      <c r="D546">
+        <v>27.997</v>
+      </c>
+      <c r="E546">
+        <v>73.504</v>
+      </c>
+      <c r="F546">
+        <v>1401.664</v>
+      </c>
+      <c r="G546">
+        <v>1094.108</v>
+      </c>
+      <c r="H546">
+        <v>1617.146</v>
+      </c>
+      <c r="I546">
+        <v>2711.254</v>
+      </c>
+      <c r="J546">
+        <v>4112.918</v>
+      </c>
+      <c r="K546">
+        <v>0</v>
+      </c>
+      <c r="L546">
+        <v>58951.924</v>
+      </c>
+      <c r="M546">
+        <v>63138.346</v>
+      </c>
+    </row>
+    <row r="547" spans="1:13">
+      <c r="A547" s="6">
+        <v>42917</v>
+      </c>
+      <c r="B547" t="s">
+        <v>19</v>
+      </c>
+      <c r="C547">
+        <v>53.309</v>
+      </c>
+      <c r="D547">
+        <v>16.546</v>
+      </c>
+      <c r="E547">
+        <v>69.855</v>
+      </c>
+      <c r="F547">
+        <v>1494.46</v>
+      </c>
+      <c r="G547">
+        <v>1047.123</v>
+      </c>
+      <c r="H547">
+        <v>1838.301</v>
+      </c>
+      <c r="I547">
+        <v>2885.424</v>
+      </c>
+      <c r="J547">
+        <v>4379.884</v>
+      </c>
+      <c r="K547">
+        <v>0</v>
+      </c>
+      <c r="L547">
+        <v>69900.111</v>
+      </c>
+      <c r="M547">
+        <v>74349.85</v>
+      </c>
+    </row>
+    <row r="548" spans="1:13">
+      <c r="A548" s="6">
+        <v>42948</v>
+      </c>
+      <c r="B548" t="s">
+        <v>19</v>
+      </c>
+      <c r="C548">
+        <v>48.549</v>
+      </c>
+      <c r="D548">
+        <v>15.069</v>
+      </c>
+      <c r="E548">
+        <v>63.618</v>
+      </c>
+      <c r="F548">
+        <v>1528.056</v>
+      </c>
+      <c r="G548">
+        <v>1064.994</v>
+      </c>
+      <c r="H548">
+        <v>1807.254</v>
+      </c>
+      <c r="I548">
+        <v>2872.248</v>
+      </c>
+      <c r="J548">
+        <v>4400.304</v>
+      </c>
+      <c r="K548">
+        <v>0</v>
+      </c>
+      <c r="L548">
+        <v>65933.994</v>
+      </c>
+      <c r="M548">
+        <v>70397.916</v>
+      </c>
+    </row>
+    <row r="549" spans="1:13">
+      <c r="A549" s="6">
+        <v>42979</v>
+      </c>
+      <c r="B549" t="s">
+        <v>19</v>
+      </c>
+      <c r="C549">
+        <v>47.069</v>
+      </c>
+      <c r="D549">
+        <v>14.609</v>
+      </c>
+      <c r="E549">
+        <v>61.678</v>
+      </c>
+      <c r="F549">
+        <v>1468.767</v>
+      </c>
+      <c r="G549">
+        <v>1030.015</v>
+      </c>
+      <c r="H549">
+        <v>1809.249</v>
+      </c>
+      <c r="I549">
+        <v>2839.264</v>
+      </c>
+      <c r="J549">
+        <v>4308.031</v>
+      </c>
+      <c r="K549">
+        <v>0</v>
+      </c>
+      <c r="L549">
+        <v>54779.784</v>
+      </c>
+      <c r="M549">
+        <v>59149.493</v>
+      </c>
+    </row>
+    <row r="550" spans="1:13">
+      <c r="A550" s="6">
+        <v>43009</v>
+      </c>
+      <c r="B550" t="s">
+        <v>19</v>
+      </c>
+      <c r="C550">
+        <v>42.669</v>
+      </c>
+      <c r="D550">
+        <v>37.703</v>
+      </c>
+      <c r="E550">
+        <v>80.372</v>
+      </c>
+      <c r="F550">
+        <v>1469.57</v>
+      </c>
+      <c r="G550">
+        <v>1149.103</v>
+      </c>
+      <c r="H550">
+        <v>1641.732</v>
+      </c>
+      <c r="I550">
+        <v>2790.835</v>
+      </c>
+      <c r="J550">
+        <v>4260.405</v>
+      </c>
+      <c r="K550">
+        <v>0</v>
+      </c>
+      <c r="L550">
+        <v>50214.467</v>
+      </c>
+      <c r="M550">
+        <v>54555.244</v>
+      </c>
+    </row>
+    <row r="551" spans="1:13">
+      <c r="A551" s="6">
+        <v>43040</v>
+      </c>
+      <c r="B551" t="s">
+        <v>19</v>
+      </c>
+      <c r="C551">
+        <v>49.578</v>
+      </c>
+      <c r="D551">
+        <v>43.808</v>
+      </c>
+      <c r="E551">
+        <v>93.386</v>
+      </c>
+      <c r="F551">
+        <v>1456.863</v>
+      </c>
+      <c r="G551">
+        <v>1142.217</v>
+      </c>
+      <c r="H551">
+        <v>1650.271</v>
+      </c>
+      <c r="I551">
+        <v>2792.488</v>
+      </c>
+      <c r="J551">
+        <v>4249.351</v>
+      </c>
+      <c r="K551">
+        <v>0</v>
+      </c>
+      <c r="L551">
+        <v>50992.13</v>
+      </c>
+      <c r="M551">
+        <v>55334.867</v>
+      </c>
+    </row>
+    <row r="552" spans="1:13">
+      <c r="A552" s="6">
+        <v>43070</v>
+      </c>
+      <c r="B552" t="s">
+        <v>19</v>
+      </c>
+      <c r="C552">
+        <v>61.661</v>
+      </c>
+      <c r="D552">
+        <v>54.486</v>
+      </c>
+      <c r="E552">
+        <v>116.147</v>
+      </c>
+      <c r="F552">
+        <v>1558.946</v>
+      </c>
+      <c r="G552">
+        <v>1180.736</v>
+      </c>
+      <c r="H552">
+        <v>1605.369</v>
+      </c>
+      <c r="I552">
+        <v>2786.105</v>
+      </c>
+      <c r="J552">
+        <v>4345.051</v>
+      </c>
+      <c r="K552">
+        <v>0</v>
+      </c>
+      <c r="L552">
+        <v>58388.345</v>
+      </c>
+      <c r="M552">
+        <v>62849.543</v>
+      </c>
+    </row>
+    <row r="553" spans="1:13">
+      <c r="A553" s="6">
+        <v>43101</v>
+      </c>
+      <c r="B553" t="s">
+        <v>19</v>
+      </c>
+      <c r="C553">
+        <v>68.861</v>
+      </c>
+      <c r="D553">
+        <v>35.059</v>
+      </c>
+      <c r="E553">
+        <v>103.92</v>
+      </c>
+      <c r="F553">
+        <v>1689.106</v>
+      </c>
+      <c r="G553">
+        <v>1269.77</v>
+      </c>
+      <c r="H553">
+        <v>1667.075</v>
+      </c>
+      <c r="I553">
+        <v>2936.845</v>
+      </c>
+      <c r="J553">
+        <v>4625.951</v>
+      </c>
+      <c r="K553">
+        <v>0</v>
+      </c>
+      <c r="L553">
+        <v>64650.176</v>
+      </c>
+      <c r="M553">
+        <v>69380.047</v>
+      </c>
+    </row>
+    <row r="554" spans="1:13">
+      <c r="A554" s="6">
+        <v>43132</v>
+      </c>
+      <c r="B554" t="s">
+        <v>19</v>
+      </c>
+      <c r="C554">
+        <v>53.112</v>
+      </c>
+      <c r="D554">
+        <v>50.81</v>
+      </c>
+      <c r="E554">
+        <v>103.922</v>
+      </c>
+      <c r="F554">
+        <v>1388.187</v>
+      </c>
+      <c r="G554">
+        <v>1131.822</v>
+      </c>
+      <c r="H554">
+        <v>1729.148</v>
+      </c>
+      <c r="I554">
+        <v>2860.97</v>
+      </c>
+      <c r="J554">
+        <v>4249.157</v>
+      </c>
+      <c r="K554">
+        <v>0</v>
+      </c>
+      <c r="L554">
+        <v>45823.067</v>
+      </c>
+      <c r="M554">
+        <v>50176.146</v>
+      </c>
+    </row>
+    <row r="555" spans="1:13">
+      <c r="A555" s="6">
+        <v>43160</v>
+      </c>
+      <c r="B555" t="s">
+        <v>19</v>
+      </c>
+      <c r="C555">
+        <v>50.608</v>
+      </c>
+      <c r="D555">
+        <v>7.14</v>
+      </c>
+      <c r="E555">
+        <v>57.748</v>
+      </c>
+      <c r="F555">
+        <v>1113.576</v>
+      </c>
+      <c r="G555">
+        <v>1169.107</v>
+      </c>
+      <c r="H555">
+        <v>1610.478</v>
+      </c>
+      <c r="I555">
+        <v>2779.585</v>
+      </c>
+      <c r="J555">
+        <v>3893.161</v>
+      </c>
+      <c r="K555">
+        <v>0</v>
+      </c>
+      <c r="L555">
+        <v>44495.503</v>
+      </c>
+      <c r="M555">
+        <v>48446.411</v>
       </c>
     </row>
   </sheetData>
@@ -22373,7 +22906,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -25262,37 +25795,78 @@
         <v>19</v>
       </c>
       <c r="C80">
-        <v>691.92</v>
+        <v>682.895</v>
       </c>
       <c r="D80">
-        <v>489.98</v>
+        <v>499.814</v>
       </c>
       <c r="E80">
-        <v>1181.9</v>
+        <v>1182.709</v>
       </c>
       <c r="F80">
         <v>16484.708</v>
       </c>
       <c r="G80">
-        <v>14302.087</v>
+        <v>14720.22</v>
       </c>
       <c r="H80">
-        <v>20257.189</v>
+        <v>20128.567</v>
       </c>
       <c r="I80">
-        <v>34559.276</v>
+        <v>34848.787</v>
       </c>
       <c r="J80">
-        <v>51043.984</v>
+        <v>51333.495</v>
       </c>
       <c r="K80">
         <v>0</v>
       </c>
       <c r="L80">
-        <v>677274.728</v>
+        <v>678554.486</v>
       </c>
       <c r="M80">
-        <v>729500.612</v>
+        <v>731070.69</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
+      <c r="A81" s="7">
+        <v>2017</v>
+      </c>
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81">
+        <v>607.058</v>
+      </c>
+      <c r="D81">
+        <v>454.085</v>
+      </c>
+      <c r="E81">
+        <v>1061.143</v>
+      </c>
+      <c r="F81">
+        <v>17537.663</v>
+      </c>
+      <c r="G81">
+        <v>13424.174</v>
+      </c>
+      <c r="H81">
+        <v>20188.749</v>
+      </c>
+      <c r="I81">
+        <v>33612.923</v>
+      </c>
+      <c r="J81">
+        <v>51150.586</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>664749.129</v>
+      </c>
+      <c r="M81">
+        <v>716960.858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>